<commit_message>
Added Clay county AR
</commit_message>
<xml_diff>
--- a/data_in/Countys_smartrice.xlsx
+++ b/data_in/Countys_smartrice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trubin\Desktop\Landviser LLC\git repos\soils-ssurgo\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236B0CBF-4794-4A35-85A9-0508AA91A922}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81183A7D-2483-4FDA-857B-D49187C1C628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11604" windowHeight="8766" xr2:uid="{E6DDC3F0-D229-4B89-904C-5539883CB6A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="29">
   <si>
     <t>NAME</t>
   </si>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C234B32-A077-4C51-96AD-0BBB8A673DC9}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" activeCellId="2" sqref="A11:D12 A6:D6 A20:D20"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -569,16 +569,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>5021</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Jupiter with unzipper and zip+output files were added
</commit_message>
<xml_diff>
--- a/data_in/Countys_smartrice.xlsx
+++ b/data_in/Countys_smartrice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trubin\Desktop\Landviser LLC\git repos\soils-ssurgo\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81183A7D-2483-4FDA-857B-D49187C1C628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77BDFAC-154E-4AAF-BA80-6599FBB9F4F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11604" windowHeight="8766" xr2:uid="{E6DDC3F0-D229-4B89-904C-5539883CB6A5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>NAME</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D7" sqref="A7:D7"/>
+      <selection activeCell="D17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -499,58 +499,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>5067</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>5147</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>5035</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5093</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -583,44 +583,44 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>29181</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>29207</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>29143</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -653,100 +653,100 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>48039</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>29201</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>48481</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>48473</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>48201</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>5037</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>5111</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>